<commit_message>
fix bug export documents
</commit_message>
<xml_diff>
--- a/public/export/group_list_cn/group_list_cn_tmp.xlsx
+++ b/public/export/group_list_cn/group_list_cn_tmp.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames/>
+  <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="cqxquPAuvWcxdXwm359tepmiSox2z3kThh4ZyUuwSCE="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CÔNG TY TNHH VẠN SỰ THÔNG</t>
   </si>
@@ -36,88 +41,41 @@
   <si>
     <t>通行证号</t>
   </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>NGUYEN THI KIM DUNG</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>19631222</t>
-  </si>
-  <si>
-    <t>PHAM THE NHAN</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>19561031</t>
-  </si>
-  <si>
-    <t>NGUYEN NHU HAI</t>
-  </si>
-  <si>
-    <t>20020521</t>
-  </si>
-  <si>
-    <t>NGUYEN CAM TRIEU</t>
-  </si>
-  <si>
-    <t>19790528</t>
-  </si>
-  <si>
-    <t>NGUYEN BAO THY</t>
-  </si>
-  <si>
-    <t>20100115</t>
-  </si>
-  <si>
-    <t>NGUYEN TRUONG SON</t>
-  </si>
-  <si>
-    <t>19740326</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyymmdd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
-      <sz val="11"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="15.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="15.0"/>
       <color theme="1"/>
-      <sz val="15"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <sz val="15"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <color theme="1"/>
-      <sz val="15"/>
       <name val="SimSun"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
-      <scheme val="minor"/>
-      <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -126,17 +84,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -150,57 +102,53 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="1" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="1" vertical="center" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,24 +346,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="14.43"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="2.14" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="9.71" customWidth="1"/>
-    <col min="5" max="7" width="18.57" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="2.14"/>
+    <col customWidth="1" min="2" max="2" width="11.0"/>
+    <col customWidth="1" min="3" max="3" width="34.0"/>
+    <col customWidth="1" min="4" max="4" width="9.71"/>
+    <col customWidth="1" min="5" max="7" width="18.57"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" ht="12.0" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -424,38 +371,22 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4">
       <c r="A4" s="1"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -464,7 +395,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" ht="20.25" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>2</v>
@@ -485,121 +416,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" ht="20.25" customHeight="1">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" ht="20.25" customHeight="1">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" ht="20.25" customHeight="1">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" ht="20.25" customHeight="1">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" ht="20.25" customHeight="1">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" ht="20.25" customHeight="1">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -607,7 +472,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" ht="20.25" customHeight="1">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -615,7 +480,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" ht="20.25" customHeight="1">
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -623,7 +488,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" ht="20.25" customHeight="1">
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -631,7 +496,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" ht="20.25" customHeight="1">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -639,7 +504,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" ht="20.25" customHeight="1">
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -647,7 +512,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" ht="20.25" customHeight="1">
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -655,7 +520,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" ht="20.25" customHeight="1">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -663,7 +528,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" ht="20.25" customHeight="1">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -671,7 +536,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" ht="20.25" customHeight="1">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -679,7 +544,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" ht="20.25" customHeight="1">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -687,7 +552,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" ht="20.25" customHeight="1">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -695,7 +560,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" ht="20.25" customHeight="1">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -703,7 +568,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" ht="20.25" customHeight="1">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -711,7 +576,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" ht="20.25" customHeight="1">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -719,7 +584,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" ht="20.25" customHeight="1">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -727,7 +592,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" ht="20.25" customHeight="1">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -735,7 +600,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" ht="20.25" customHeight="1">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -743,7 +608,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" ht="20.25" customHeight="1">
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -751,7 +616,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" ht="20.25" customHeight="1">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -759,7 +624,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" ht="20.25" customHeight="1">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -767,7 +632,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" ht="20.25" customHeight="1">
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -775,7 +640,7 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" ht="20.25" customHeight="1">
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -783,7 +648,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" ht="20.25" customHeight="1">
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -791,7 +656,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" ht="20.25" customHeight="1">
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -799,7 +664,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" ht="20.25" customHeight="1">
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -807,7 +672,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" ht="20.25" customHeight="1">
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -815,7 +680,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" ht="20.25" customHeight="1">
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -823,7 +688,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" ht="20.25" customHeight="1">
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -831,7 +696,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" ht="20.25" customHeight="1">
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -839,7 +704,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" ht="20.25" customHeight="1">
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -847,7 +712,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" ht="20.25" customHeight="1">
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
@@ -855,7 +720,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" ht="20.25" customHeight="1">
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -863,7 +728,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" ht="20.25" customHeight="1">
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
@@ -871,7 +736,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" ht="20.25" customHeight="1">
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
@@ -879,7 +744,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" ht="20.25" customHeight="1">
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -887,7 +752,7 @@
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" ht="20.25" customHeight="1">
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
@@ -895,7 +760,7 @@
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" ht="20.25" customHeight="1">
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -903,7 +768,7 @@
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" ht="20.25" customHeight="1">
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -911,7 +776,7 @@
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" ht="20.25" customHeight="1">
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -919,7 +784,7 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" ht="20.25" customHeight="1">
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -927,7 +792,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" ht="20.25" customHeight="1">
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -935,7 +800,7 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
     </row>
-    <row r="55" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" ht="20.25" customHeight="1">
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -943,7 +808,7 @@
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" ht="20.25" customHeight="1">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -951,7 +816,7 @@
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
     </row>
-    <row r="57" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" ht="20.25" customHeight="1">
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -959,7 +824,7 @@
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
     </row>
-    <row r="58" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" ht="20.25" customHeight="1">
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -967,7 +832,7 @@
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" ht="20.25" customHeight="1">
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -975,7 +840,7 @@
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
     </row>
-    <row r="60" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" ht="20.25" customHeight="1">
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -983,7 +848,7 @@
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" ht="20.25" customHeight="1">
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -991,7 +856,7 @@
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" ht="20.25" customHeight="1">
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -999,7 +864,7 @@
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
     </row>
-    <row r="63" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" ht="20.25" customHeight="1">
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -1007,7 +872,7 @@
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
     </row>
-    <row r="64" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" ht="20.25" customHeight="1">
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -1015,7 +880,7 @@
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
     </row>
-    <row r="65" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" ht="20.25" customHeight="1">
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -1023,7 +888,7 @@
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
     </row>
-    <row r="66" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" ht="20.25" customHeight="1">
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
@@ -1031,7 +896,7 @@
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
     </row>
-    <row r="67" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" ht="20.25" customHeight="1">
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -1039,7 +904,7 @@
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
     </row>
-    <row r="68" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" ht="20.25" customHeight="1">
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -1047,7 +912,7 @@
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
     </row>
-    <row r="69" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" ht="20.25" customHeight="1">
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -1055,7 +920,7 @@
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
     </row>
-    <row r="70" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" ht="20.25" customHeight="1">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -1063,7 +928,7 @@
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" ht="20.25" customHeight="1">
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
@@ -1071,7 +936,7 @@
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" ht="20.25" customHeight="1">
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -1079,7 +944,7 @@
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" ht="20.25" customHeight="1">
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
@@ -1087,7 +952,7 @@
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" ht="20.25" customHeight="1">
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -1095,7 +960,7 @@
       <c r="F74" s="10"/>
       <c r="G74" s="10"/>
     </row>
-    <row r="75" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" ht="20.25" customHeight="1">
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -1103,7 +968,7 @@
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
     </row>
-    <row r="76" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" ht="20.25" customHeight="1">
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
@@ -1111,7 +976,7 @@
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
     </row>
-    <row r="77" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" ht="20.25" customHeight="1">
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
@@ -1119,7 +984,7 @@
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
     </row>
-    <row r="78" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" ht="20.25" customHeight="1">
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
@@ -1127,7 +992,7 @@
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
     </row>
-    <row r="79" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" ht="20.25" customHeight="1">
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
@@ -1135,7 +1000,7 @@
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
     </row>
-    <row r="80" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" ht="20.25" customHeight="1">
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
@@ -1143,7 +1008,7 @@
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
     </row>
-    <row r="81" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" ht="20.25" customHeight="1">
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
@@ -1151,7 +1016,7 @@
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
     </row>
-    <row r="82" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" ht="20.25" customHeight="1">
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
@@ -1159,7 +1024,7 @@
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
     </row>
-    <row r="83" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" ht="20.25" customHeight="1">
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
@@ -1167,7 +1032,7 @@
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
     </row>
-    <row r="84" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" ht="20.25" customHeight="1">
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
@@ -1175,7 +1040,7 @@
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
     </row>
-    <row r="85" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" ht="20.25" customHeight="1">
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
@@ -1183,7 +1048,7 @@
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
     </row>
-    <row r="86" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" ht="20.25" customHeight="1">
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
@@ -1191,7 +1056,7 @@
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
     </row>
-    <row r="87" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" ht="20.25" customHeight="1">
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
@@ -1199,7 +1064,7 @@
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
     </row>
-    <row r="88" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" ht="20.25" customHeight="1">
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
@@ -1207,7 +1072,7 @@
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" ht="20.25" customHeight="1">
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
@@ -1215,7 +1080,7 @@
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" ht="20.25" customHeight="1">
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
       <c r="D90" s="10"/>
@@ -1223,7 +1088,7 @@
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
     </row>
-    <row r="91" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" ht="20.25" customHeight="1">
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
@@ -1231,7 +1096,7 @@
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
     </row>
-    <row r="92" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" ht="20.25" customHeight="1">
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
@@ -1239,7 +1104,7 @@
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
     </row>
-    <row r="93" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" ht="20.25" customHeight="1">
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
@@ -1247,7 +1112,7 @@
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
     </row>
-    <row r="94" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" ht="20.25" customHeight="1">
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
@@ -1255,7 +1120,7 @@
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
     </row>
-    <row r="95" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" ht="20.25" customHeight="1">
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
@@ -1263,7 +1128,7 @@
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
     </row>
-    <row r="96" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" ht="20.25" customHeight="1">
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
@@ -1271,7 +1136,7 @@
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
     </row>
-    <row r="97" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" ht="20.25" customHeight="1">
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
@@ -1279,7 +1144,7 @@
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
     </row>
-    <row r="98" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" ht="20.25" customHeight="1">
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
@@ -1287,7 +1152,7 @@
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
     </row>
-    <row r="99" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" ht="20.25" customHeight="1">
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10"/>
@@ -1295,7 +1160,7 @@
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
     </row>
-    <row r="100" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" ht="20.25" customHeight="1">
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
       <c r="D100" s="10"/>
@@ -1303,7 +1168,7 @@
       <c r="F100" s="10"/>
       <c r="G100" s="10"/>
     </row>
-    <row r="101" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" ht="20.25" customHeight="1">
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
@@ -1311,7 +1176,7 @@
       <c r="F101" s="10"/>
       <c r="G101" s="10"/>
     </row>
-    <row r="102" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" ht="20.25" customHeight="1">
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
@@ -1319,7 +1184,7 @@
       <c r="F102" s="10"/>
       <c r="G102" s="10"/>
     </row>
-    <row r="103" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" ht="20.25" customHeight="1">
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
       <c r="D103" s="10"/>
@@ -1327,7 +1192,7 @@
       <c r="F103" s="10"/>
       <c r="G103" s="10"/>
     </row>
-    <row r="104" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" ht="20.25" customHeight="1">
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
       <c r="D104" s="10"/>
@@ -1335,7 +1200,7 @@
       <c r="F104" s="10"/>
       <c r="G104" s="10"/>
     </row>
-    <row r="105" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" ht="20.25" customHeight="1">
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
       <c r="D105" s="10"/>
@@ -1343,7 +1208,7 @@
       <c r="F105" s="10"/>
       <c r="G105" s="10"/>
     </row>
-    <row r="106" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" ht="20.25" customHeight="1">
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="D106" s="10"/>
@@ -1351,7 +1216,7 @@
       <c r="F106" s="10"/>
       <c r="G106" s="10"/>
     </row>
-    <row r="107" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" ht="20.25" customHeight="1">
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="10"/>
@@ -1359,7 +1224,7 @@
       <c r="F107" s="10"/>
       <c r="G107" s="10"/>
     </row>
-    <row r="108" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" ht="20.25" customHeight="1">
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="D108" s="10"/>
@@ -1367,7 +1232,7 @@
       <c r="F108" s="10"/>
       <c r="G108" s="10"/>
     </row>
-    <row r="109" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" ht="20.25" customHeight="1">
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="10"/>
@@ -1375,7 +1240,7 @@
       <c r="F109" s="10"/>
       <c r="G109" s="10"/>
     </row>
-    <row r="110" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" ht="20.25" customHeight="1">
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
       <c r="D110" s="10"/>
@@ -1383,64 +1248,895 @@
       <c r="F110" s="10"/>
       <c r="G110" s="10"/>
     </row>
-    <row r="111" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="10"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="10"/>
-      <c r="F111" s="10"/>
-      <c r="G111" s="10"/>
-    </row>
-    <row r="112" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="10"/>
-      <c r="F112" s="10"/>
-      <c r="G112" s="10"/>
-    </row>
-    <row r="113" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="10"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="10"/>
-      <c r="F113" s="10"/>
-      <c r="G113" s="10"/>
-    </row>
-    <row r="114" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="10"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="10"/>
-      <c r="G114" s="10"/>
-    </row>
-    <row r="115" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="10"/>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="10"/>
-      <c r="F115" s="10"/>
-      <c r="G115" s="10"/>
-    </row>
-    <row r="116" ht="20.25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="10"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
-      <c r="E116" s="10"/>
-      <c r="F116" s="10"/>
-      <c r="G116" s="10"/>
-    </row>
-    <row r="117" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="20.25" customHeight="1"/>
+    <row r="112" ht="20.25" customHeight="1"/>
+    <row r="113" ht="20.25" customHeight="1"/>
+    <row r="114" ht="20.25" customHeight="1"/>
+    <row r="115" ht="20.25" customHeight="1"/>
+    <row r="116" ht="20.25" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G4"/>
   </mergeCells>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>